<commit_message>
Ongoing testing of preemptive multitasking
</commit_message>
<xml_diff>
--- a/Resources/virtualizaton.xlsx
+++ b/Resources/virtualizaton.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Saved registers</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>ESP</t>
-  </si>
-  <si>
-    <t>PC</t>
   </si>
   <si>
     <t>downto</t>
@@ -431,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M15"/>
+  <dimension ref="A2:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,22 +447,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <f>B3-1</f>
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -473,46 +470,46 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>32</v>
       </c>
       <c r="C4">
-        <f>C3+B4</f>
-        <v>51</v>
+        <f t="shared" ref="C4:C8" si="0">C3+B4</f>
+        <v>63</v>
       </c>
       <c r="D4">
-        <f>D3+B4</f>
+        <f t="shared" ref="D4:D8" si="1">D3+B4</f>
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C9" si="0">C4+B5</f>
-        <v>83</v>
+        <f t="shared" si="0"/>
+        <v>71</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D9" si="1">D4+B5</f>
+        <f>C4+1</f>
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
@@ -521,14 +518,14 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
@@ -537,14 +534,14 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
@@ -552,69 +549,53 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>115</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="1"/>
+      <c r="B9" s="3">
+        <f>SUM(B3:B8)</f>
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
-        <f>SUM(B3:B9)</f>
-        <v>116</v>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B14">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
-      </c>
-      <c r="M14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
         <v>11</v>
-      </c>
-      <c r="B15">
-        <v>6</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>